<commit_message>
updating WHI data layers, added a new folder layers_wh for storing final wh data layers
</commit_message>
<xml_diff>
--- a/prep_whi/CS_CP_HAB/wetlands/ccap_wetlands_wh.xlsx
+++ b/prep_whi/CS_CP_HAB/wetlands/ccap_wetlands_wh.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/WHI/prep_whi/CS_CP_HAB/wetlands/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="5900" windowWidth="21580" windowHeight="7980"/>
+    <workbookView xWindow="6220" yWindow="5900" windowWidth="21580" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="south" sheetId="1" r:id="rId1"/>
-    <sheet name="north" sheetId="2" r:id="rId2"/>
+    <sheet name="south_2010" sheetId="1" r:id="rId1"/>
+    <sheet name="north_2010" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,10 +429,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -535,11 +535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>